<commit_message>
update chart in YUDI's file
</commit_message>
<xml_diff>
--- a/CapabilityMatrix/QAcapability_于荻.xlsx
+++ b/CapabilityMatrix/QAcapability_于荻.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Exploratory Testing</t>
   </si>
@@ -226,13 +226,16 @@
   </si>
   <si>
     <t>Mobile Testing</t>
+  </si>
+  <si>
+    <t>OVERALL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -261,6 +264,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -280,7 +299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -318,20 +337,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -369,19 +400,8 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fundamental Technics</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>current</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$A$2:$A$12</c:f>
@@ -472,9 +492,6 @@
           <c:tx>
             <c:v>nextphase</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$C$2:$C$12</c:f>
@@ -526,11 +543,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="107374080"/>
-        <c:axId val="107375616"/>
+        <c:axId val="91382144"/>
+        <c:axId val="91383680"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="107374080"/>
+        <c:axId val="91382144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +558,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107375616"/>
+        <c:crossAx val="91383680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -549,9 +566,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107375616"/>
+        <c:axId val="91383680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -560,7 +578,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107374080"/>
+        <c:crossAx val="91382144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -596,10 +614,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -610,19 +624,8 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$A$135</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Process Improve</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>current</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$A$136:$A$140</c:f>
@@ -649,6 +652,60 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$B$136:$B$140</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3 months</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$136:$A$140</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Agile</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Scrum/Kanban/XP</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bug Analyse</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Risk Manage</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DevOps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$136:$C$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -679,11 +736,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142758656"/>
-        <c:axId val="142760192"/>
+        <c:axId val="94403200"/>
+        <c:axId val="94417280"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="142758656"/>
+        <c:axId val="94403200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,7 +751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142760192"/>
+        <c:crossAx val="94417280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -702,9 +759,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142760192"/>
+        <c:axId val="94417280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -713,7 +771,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142758656"/>
+        <c:crossAx val="94403200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -768,6 +826,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>current</c:v>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -823,6 +884,93 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3 months</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet2!$A$1,Sheet2!$A$17,Sheet2!$A$31,Sheet2!$A$46,Sheet2!$A$63,Sheet2!$A$76,Sheet2!$A$95,Sheet2!$A$109,Sheet2!$A$122,Sheet2!$A$135)</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Fundamental Technics</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Automation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Test Method</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Test Case Design</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test Strategy</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Test Technics</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Requirement Analyse</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Business Knowledge</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Communication</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Process Improve</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet2!$C$1,Sheet2!$C$17,Sheet2!$C$31,Sheet2!$C$46,Sheet2!$C$63,Sheet2!$C$76,Sheet2!$C$95,Sheet2!$C$109,Sheet2!$C$122,Sheet2!$C$135)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.2727272727272729</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.8</c:v>
@@ -857,11 +1005,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116049024"/>
-        <c:axId val="128544768"/>
+        <c:axId val="94445568"/>
+        <c:axId val="94447104"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="116049024"/>
+        <c:axId val="94445568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,7 +1020,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128544768"/>
+        <c:crossAx val="94447104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -880,9 +1028,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128544768"/>
+        <c:axId val="94447104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -891,7 +1040,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116049024"/>
+        <c:crossAx val="94445568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -927,10 +1076,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -941,19 +1086,8 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$A$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Automation</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>current</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$A$18:$A$22</c:f>
@@ -980,6 +1114,60 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$B$18:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3 months</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$18:$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Automation Strategy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Coding</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Toolset</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Refactor&amp;Case manage</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Framework Design</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$18:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1010,11 +1198,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69229952"/>
-        <c:axId val="87778432"/>
+        <c:axId val="91399680"/>
+        <c:axId val="91401216"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="69229952"/>
+        <c:axId val="91399680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,7 +1213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87778432"/>
+        <c:crossAx val="91401216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1033,9 +1221,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87778432"/>
+        <c:axId val="91401216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1044,7 +1233,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69229952"/>
+        <c:crossAx val="91399680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1090,19 +1279,8 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$A$31</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Test Method</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>current</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$A$32:$A$36</c:f>
@@ -1155,11 +1333,31 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>nextphase</c:v>
+            <c:v>3 months</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$32:$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Component/Integration Test</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UT/TDD</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Regression Test</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Alpha&amp;Beta</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>System Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$C$32:$C$36</c:f>
@@ -1193,11 +1391,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115984256"/>
-        <c:axId val="115985792"/>
+        <c:axId val="93536256"/>
+        <c:axId val="93537792"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="115984256"/>
+        <c:axId val="93536256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1208,7 +1406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115985792"/>
+        <c:crossAx val="93537792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1216,9 +1414,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115985792"/>
+        <c:axId val="93537792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1227,7 +1426,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115984256"/>
+        <c:crossAx val="93536256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1263,10 +1462,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1277,19 +1472,8 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$A$46</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Test Case Design</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>current</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$A$47:$A$55</c:f>
@@ -1328,6 +1512,84 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$B$47:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3 months</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$47:$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Boundary Value</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Equivalence Class</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>State Transition Diagrams</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>User Scenario</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Error Guessing</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Statement Coverage</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Branch Coverage</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Path Coverage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$47:$C$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1370,11 +1632,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="112092672"/>
-        <c:axId val="112094592"/>
+        <c:axId val="93574272"/>
+        <c:axId val="93575808"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="112092672"/>
+        <c:axId val="93574272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1385,7 +1647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112094592"/>
+        <c:crossAx val="93575808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1393,9 +1655,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112094592"/>
+        <c:axId val="93575808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1404,7 +1667,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112092672"/>
+        <c:crossAx val="93574272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1440,10 +1703,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1454,19 +1713,8 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$A$63</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Test Strategy</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>current</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$A$64:$A$68</c:f>
@@ -1493,6 +1741,60 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$B$64:$B$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3 months</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$64:$A$68</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Test Schedule</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Test Levels</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Test Tools</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Test Priority</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test Approach</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$64:$C$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1523,11 +1825,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113252992"/>
-        <c:axId val="113287552"/>
+        <c:axId val="93946624"/>
+        <c:axId val="93948160"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="113252992"/>
+        <c:axId val="93946624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1538,7 +1840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113287552"/>
+        <c:crossAx val="93948160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1546,9 +1848,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113287552"/>
+        <c:axId val="93948160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1557,7 +1860,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113252992"/>
+        <c:crossAx val="93946624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1593,10 +1896,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1607,15 +1906,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$A$76</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Test Technics</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>current</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -1658,6 +1949,87 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$B$77:$B$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3 month2</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$77:$A$85</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Security Testing</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Performance Testing</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Web Testing</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mobile Testing</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Usability Testing</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Compatibility Testing</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Localisation Testing</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Exploratory Testing</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Embedded Testing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$77:$C$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1700,11 +2072,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="128435328"/>
-        <c:axId val="128436864"/>
+        <c:axId val="93964544"/>
+        <c:axId val="93970432"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="128435328"/>
+        <c:axId val="93964544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,7 +2087,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128436864"/>
+        <c:crossAx val="93970432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1723,9 +2095,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128436864"/>
+        <c:axId val="93970432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1734,7 +2107,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128435328"/>
+        <c:crossAx val="93964544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1770,10 +2143,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1784,19 +2153,8 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$A$95</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Requirement Analyse</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>current</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$A$96:$A$99</c:f>
@@ -1820,6 +2178,54 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$B$96:$B$99</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3 month</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$96:$A$99</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Requirement understand</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Requirement clarity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Write AC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Specific as QA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$96:$C$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1847,11 +2253,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="128472960"/>
-        <c:axId val="128474496"/>
+        <c:axId val="94265344"/>
+        <c:axId val="94266880"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="128472960"/>
+        <c:axId val="94265344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1862,7 +2268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128474496"/>
+        <c:crossAx val="94266880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1870,9 +2276,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128474496"/>
+        <c:axId val="94266880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1881,7 +2288,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128472960"/>
+        <c:crossAx val="94265344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1976,11 +2383,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="128563456"/>
-        <c:axId val="128579072"/>
+        <c:axId val="94295552"/>
+        <c:axId val="94297088"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="128563456"/>
+        <c:axId val="94295552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1991,7 +2398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128579072"/>
+        <c:crossAx val="94297088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1999,9 +2406,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128579072"/>
+        <c:axId val="94297088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2010,7 +2418,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128563456"/>
+        <c:crossAx val="94295552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2046,10 +2454,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2060,19 +2464,8 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$A$122</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Communication</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>current</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$A$123:$A$127</c:f>
@@ -2099,6 +2492,60 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$B$123:$B$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3 months</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$123:$A$127</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Ask questions</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>logical thinking</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>listen to others</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Express idea</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Team work</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$123:$C$127</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2129,11 +2576,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142761984"/>
-        <c:axId val="142763520"/>
+        <c:axId val="94382720"/>
+        <c:axId val="94392704"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="142761984"/>
+        <c:axId val="94382720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2144,7 +2591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142763520"/>
+        <c:crossAx val="94392704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2152,9 +2599,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142763520"/>
+        <c:axId val="94392704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2163,7 +2611,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142761984"/>
+        <c:crossAx val="94382720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2253,14 +2701,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>61913</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2507,16 +2955,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>153</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>177</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2862,10 +3310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C140"/>
+  <dimension ref="A1:J154"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+      <selection activeCell="O104" sqref="O104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3662,6 +4110,12 @@
         <v>2</v>
       </c>
     </row>
+    <row r="153" spans="10:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="J153" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="154" spans="10:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>